<commit_message>
Fixed naming issues with Aerosol Optical Depth, Atmospheric Moisture and Air Temperature
</commit_message>
<xml_diff>
--- a/DarkData_Python/Rules_from_experts/X Applicability to Phenomena from experts.xlsx
+++ b/DarkData_Python/Rules_from_experts/X Applicability to Phenomena from experts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="67">
   <si>
     <t>Phenomena</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Soil Moisture</t>
   </si>
   <si>
-    <t>GRET</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -190,13 +187,13 @@
     <t>Precipitation</t>
   </si>
   <si>
-    <t>AOD</t>
+    <t>Aerosol Optical Depth</t>
   </si>
   <si>
     <t xml:space="preserve">Air Pressure </t>
   </si>
   <si>
-    <t>Air Moisture</t>
+    <t>Atmospheric Moisture</t>
   </si>
   <si>
     <t>Ozone</t>
@@ -205,7 +202,7 @@
     <t>SO2</t>
   </si>
   <si>
-    <t xml:space="preserve">air temperature </t>
+    <t xml:space="preserve">Air Temperature </t>
   </si>
   <si>
     <t>CO</t>
@@ -3774,7 +3771,7 @@
     <col customWidth="1" min="2" max="2" width="17.57"/>
     <col customWidth="1" min="3" max="3" width="20.29"/>
     <col customWidth="1" min="4" max="4" width="15.43"/>
-    <col customWidth="1" min="5" max="5" width="5.57"/>
+    <col customWidth="1" min="5" max="5" width="7.86"/>
     <col customWidth="1" min="6" max="6" width="7.29"/>
     <col customWidth="1" min="7" max="7" width="13.0"/>
     <col customWidth="1" min="8" max="8" width="5.14"/>
@@ -3895,7 +3892,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>20</v>
@@ -4111,7 +4108,7 @@
         <v>19</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>19</v>
@@ -4133,7 +4130,7 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11">
@@ -4143,7 +4140,7 @@
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -4223,49 +4220,49 @@
         <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="F2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="K2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -4273,49 +4270,49 @@
         <v>21</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="F3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="K3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
@@ -4323,49 +4320,49 @@
         <v>22</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="G4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="I4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="O4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
@@ -4373,49 +4370,49 @@
         <v>23</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="G5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="I5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K5" s="5" t="s">
+      <c r="O5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="P5" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="6">
@@ -4423,49 +4420,49 @@
         <v>25</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="G6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="I6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K6" s="5" t="s">
+      <c r="O6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="7">
@@ -4473,49 +4470,49 @@
         <v>26</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="G7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="I7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K7" s="5" t="s">
+      <c r="O7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P7" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="8">
@@ -4523,49 +4520,49 @@
         <v>27</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="G8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="I8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" s="5" t="s">
+      <c r="O8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P8" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="9">
@@ -4583,12 +4580,12 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -4670,28 +4667,28 @@
         <v>45</v>
       </c>
       <c r="R1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="U1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="V1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="W1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="X1" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="Y1" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2">
@@ -4702,33 +4699,33 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H2" s="4"/>
       <c r="Q2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="T2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="X2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
@@ -4739,33 +4736,33 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H3" s="4"/>
       <c r="Q3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="V3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="T3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="X3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -4776,35 +4773,35 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="O4" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="S4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5">
@@ -4815,24 +4812,24 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H5" s="4"/>
       <c r="J5" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="U5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
@@ -4843,39 +4840,39 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="I6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T6" s="5"/>
       <c r="U6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7">
@@ -4886,29 +4883,29 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="X7" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8">
@@ -4919,31 +4916,31 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11">
@@ -4953,22 +4950,22 @@
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>